<commit_message>
pisam working with llms
</commit_message>
<xml_diff>
--- a/src/domains/blocks/all_experiment_results-percentage-0.8.xlsx
+++ b/src/domains/blocks/all_experiment_results-percentage-0.8.xlsx
@@ -468,10 +468,10 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>0.88</v>
+        <v>0.8823529411764706</v>
       </c>
       <c r="H2">
-        <v>0.88</v>
+        <v>0.8823529411764706</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -491,13 +491,13 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>0.7777777777777778</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -520,10 +520,10 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>0.8666666666666667</v>
+        <v>0.7169811320754716</v>
       </c>
       <c r="H4">
-        <v>0.7647058823529411</v>
+        <v>0.8837209302325582</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -546,10 +546,10 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>0.7647058823529411</v>
+        <v>0.85</v>
       </c>
       <c r="H5">
-        <v>0.7647058823529411</v>
+        <v>0.6538461538461539</v>
       </c>
     </row>
   </sheetData>
@@ -611,10 +611,10 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>0.8064516129032258</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="H2">
-        <v>0.8928571428571429</v>
+        <v>0.8888888888888888</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -637,10 +637,10 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>0.8947368421052632</v>
+        <v>0.8181818181818182</v>
       </c>
       <c r="H3">
-        <v>0.8095238095238095</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -663,10 +663,10 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>0.89</v>
+        <v>0.7681159420289855</v>
       </c>
       <c r="H4">
-        <v>0.8018018018018018</v>
+        <v>0.6883116883116883</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -689,10 +689,10 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>0.7831325301204819</v>
+        <v>0.7931034482758621</v>
       </c>
       <c r="H5">
-        <v>0.7065217391304348</v>
+        <v>0.7931034482758621</v>
       </c>
     </row>
   </sheetData>
@@ -754,10 +754,10 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="H2">
-        <v>0.8852459016393442</v>
+        <v>0.7777777777777778</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -780,10 +780,10 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>0.90625</v>
+        <v>0.8</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -806,10 +806,10 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>0.875</v>
+        <v>0.8095238095238095</v>
       </c>
       <c r="H4">
-        <v>0.7777777777777778</v>
+        <v>0.8947368421052632</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -832,10 +832,10 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>0.8881987577639752</v>
+        <v>0.8823529411764706</v>
       </c>
       <c r="H5">
-        <v>0.8881987577639752</v>
+        <v>0.7894736842105263</v>
       </c>
     </row>
   </sheetData>
@@ -897,10 +897,10 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0.8121546961325967</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0.8963414634146342</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -923,10 +923,10 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>0.9016393442622952</v>
+        <v>0.8963414634146342</v>
       </c>
       <c r="H3">
-        <v>0.9016393442622952</v>
+        <v>0.8121546961325967</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -949,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0.9105691056910568</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -978,7 +978,7 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0.9017857142857144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>